<commit_message>
template gertrude et charles added
</commit_message>
<xml_diff>
--- a/students_files/template-KONGO/template-KONGO_files/planning-2 years.xlsx
+++ b/students_files/template-KONGO/template-KONGO_files/planning-2 years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BTC\Documents\Infineon\GitHub\Excellence-Program\students_files\template-KONGO\template-KONGO_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9FE2F8-C6B8-4986-8FAE-3DDB42E8FDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75351D6-4722-4921-B264-9BBB1CEB940F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1102,10 +1102,10 @@
                 <c:formatCode>_("CFA"* #,##0_);_("CFA"* \(#,##0\);_("CFA"* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2200000</c:v>
+                  <c:v>4000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7200000</c:v>
+                  <c:v>9000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1168,7 +1168,7 @@
                   <c:v>3000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7200000</c:v>
+                  <c:v>9000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1259,7 +1259,7 @@
                       <c:formatCode>_("CFA"* #,##0_);_("CFA"* \(#,##0\);_("CFA"* "-"_);_(@_)</c:formatCode>
                       <c:ptCount val="2"/>
                       <c:pt idx="0" formatCode="_(&quot;CFA&quot;* #,##0.00_);_(&quot;CFA&quot;* \(#,##0.00\);_(&quot;CFA&quot;* &quot;-&quot;??_);_(@_)">
-                        <c:v>2200000</c:v>
+                        <c:v>4000000</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>5000000</c:v>
@@ -1281,7 +1281,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Cost!$D$1</c15:sqref>
@@ -1310,7 +1310,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Cost!$B$2:$B$3</c15:sqref>
@@ -1330,7 +1330,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Cost!$D$2:$D$3</c15:sqref>
@@ -3144,8 +3144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32219F5C-0ACC-44F5-8BB6-86FC76935AA6}">
   <dimension ref="B1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3180,14 +3180,14 @@
         <v>10</v>
       </c>
       <c r="C2" s="10">
-        <v>2200000</v>
+        <v>4000000</v>
       </c>
       <c r="D2" s="11">
         <v>3000000</v>
       </c>
       <c r="E2" s="11">
         <f>C2</f>
-        <v>2200000</v>
+        <v>4000000</v>
       </c>
       <c r="F2" s="12">
         <f>D2</f>
@@ -3208,7 +3208,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="11">
         <f>E2+C3</f>
-        <v>7200000</v>
+        <v>9000000</v>
       </c>
       <c r="F3" s="5" t="e">
         <f>IF(D3="",NA(),F2+D3)</f>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="G3" s="6">
         <f>IF(ISNA(Tableau13[[#This Row],[cumulative actual cost ]]),$J$6+G2,Tableau13[[#This Row],[cumulative actual cost ]])</f>
-        <v>7200000</v>
+        <v>9000000</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>4</v>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="J4">
         <f>_xlfn.AGGREGATE(4,6,Tableau13[cumulative planned cost])</f>
-        <v>7200000</v>
+        <v>9000000</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.75">
@@ -3250,7 +3250,7 @@
       </c>
       <c r="J6">
         <f>(J4-J3)/J5</f>
-        <v>4200000</v>
+        <v>6000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>